<commit_message>
Actualización de la planificación 18/11/2024
</commit_message>
<xml_diff>
--- a/Gestión del Proyecto/Planificación.xlsx
+++ b/Gestión del Proyecto/Planificación.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
   <si>
     <t>Planificación del trabajo Completa</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Creación de la estructura de las comunicaciones entre otros SMA (XSL)</t>
   </si>
   <si>
-    <t>Comunicación entre dos agentes</t>
-  </si>
-  <si>
     <t>Almacenamiento de los agentes con los que se ha comunicado</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>5 Minutos</t>
+  </si>
+  <si>
+    <t>Comunicación entre dos agentes (Prototipo)</t>
   </si>
 </sst>
 </file>
@@ -500,9 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,17 +522,110 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,113 +633,23 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,7 +934,7 @@
   <dimension ref="C3:AD44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19:X19"/>
+      <selection activeCell="P27" sqref="P27:R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,88 +948,88 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="52"/>
     </row>
     <row r="4" spans="3:29" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
       <c r="M4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22" t="s">
+      <c r="O4" s="23"/>
+      <c r="P4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22" t="s">
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="26" t="s">
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="22" t="s">
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="22"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB4" s="23"/>
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1042,10 +1042,10 @@
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>45576</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="13">
         <v>45576</v>
       </c>
       <c r="O5" s="14"/>
@@ -1064,17 +1064,17 @@
       </c>
       <c r="W5" s="14"/>
       <c r="X5" s="14"/>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z5" s="16"/>
+      <c r="Z5" s="46"/>
       <c r="AA5" s="14"/>
       <c r="AB5" s="14"/>
-      <c r="AC5" s="7"/>
+      <c r="AC5" s="6"/>
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="14" t="s">
         <v>16</v>
       </c>
@@ -1087,38 +1087,38 @@
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>45576</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="13">
         <v>45580</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
       <c r="V6" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="16"/>
+      <c r="Z6" s="46"/>
       <c r="AA6" s="14"/>
       <c r="AB6" s="14"/>
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="14" t="s">
         <v>37</v>
       </c>
@@ -1131,10 +1131,10 @@
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>45582</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="13">
         <v>45590</v>
       </c>
       <c r="O7" s="14"/>
@@ -1153,61 +1153,61 @@
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
-      <c r="Y7" s="15" t="s">
+      <c r="Y7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z7" s="16"/>
+      <c r="Z7" s="46"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="7"/>
+      <c r="AC7" s="6"/>
     </row>
     <row r="8" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="4">
+      <c r="K8" s="21"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="3">
         <v>45576</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="22">
         <v>45589</v>
       </c>
-      <c r="O8" s="25"/>
+      <c r="O8" s="24"/>
       <c r="P8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="13"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="12"/>
-      <c r="U8" s="13"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="12"/>
       <c r="V8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="W8" s="14"/>
       <c r="X8" s="14"/>
-      <c r="Y8" s="15" t="s">
+      <c r="Y8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="16"/>
+      <c r="Z8" s="46"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
@@ -1220,10 +1220,10 @@
       </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>45576</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="13">
         <v>45590</v>
       </c>
       <c r="O9" s="14"/>
@@ -1242,66 +1242,66 @@
       </c>
       <c r="W9" s="14"/>
       <c r="X9" s="14"/>
-      <c r="Y9" s="15" t="s">
+      <c r="Y9" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z9" s="16"/>
+      <c r="Z9" s="46"/>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
-      <c r="AC9" s="7"/>
+      <c r="AC9" s="6"/>
     </row>
     <row r="10" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
+        <v>64</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="8">
+      <c r="K10" s="21"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="7">
         <v>45597</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="22">
         <v>45600</v>
       </c>
-      <c r="O10" s="25"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="13"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="12"/>
       <c r="S10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="21"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="T10" s="12"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
-      <c r="Y10" s="15" t="s">
+      <c r="Y10" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z10" s="16"/>
+      <c r="Z10" s="46"/>
       <c r="AA10" s="11"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="7"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1312,10 +1312,10 @@
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="9">
+      <c r="M11" s="8">
         <v>45577</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="13">
         <v>45608</v>
       </c>
       <c r="O11" s="14"/>
@@ -1325,25 +1325,25 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="S11" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
-      <c r="Y11" s="15" t="s">
+      <c r="Y11" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z11" s="16"/>
+      <c r="Z11" s="46"/>
       <c r="AA11" s="14"/>
       <c r="AB11" s="14"/>
     </row>
     <row r="12" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="14" t="s">
         <v>40</v>
       </c>
@@ -1352,14 +1352,14 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="9">
+      <c r="M12" s="8">
         <v>45591</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="13">
         <v>45591</v>
       </c>
       <c r="O12" s="14"/>
@@ -1369,205 +1369,205 @@
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
       <c r="S12" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
-      <c r="Y12" s="15" t="s">
+      <c r="Y12" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z12" s="16"/>
+      <c r="Z12" s="46"/>
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
     </row>
     <row r="13" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
+        <v>56</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="9">
+      <c r="K13" s="21"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="8">
         <v>45597</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="22">
         <v>45597</v>
       </c>
-      <c r="O13" s="13"/>
+      <c r="O13" s="12"/>
       <c r="P13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="T13" s="12"/>
-      <c r="U13" s="13"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="12"/>
       <c r="V13" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
-      <c r="Y13" s="15" t="s">
+      <c r="Y13" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z13" s="16"/>
+      <c r="Z13" s="46"/>
       <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
     </row>
     <row r="14" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <v>45591</v>
       </c>
-      <c r="N14" s="24">
+      <c r="N14" s="13">
         <v>45591</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="S14" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
       <c r="V14" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
-      <c r="Y14" s="15" t="s">
+      <c r="Y14" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z14" s="16"/>
+      <c r="Z14" s="46"/>
       <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
     </row>
     <row r="15" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
+        <v>73</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="9">
+      <c r="K15" s="21"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="8">
         <v>45577</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="22">
         <v>45604</v>
       </c>
-      <c r="O15" s="13"/>
+      <c r="O15" s="12"/>
       <c r="P15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="13"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="T15" s="12"/>
-      <c r="U15" s="13"/>
+        <v>65</v>
+      </c>
+      <c r="T15" s="21"/>
+      <c r="U15" s="12"/>
       <c r="V15" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="W15" s="12"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" s="21"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z15" s="16"/>
+      <c r="Z15" s="46"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="13"/>
+      <c r="AB15" s="12"/>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="9">
+      <c r="K16" s="21"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="8">
         <v>45577</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="22">
         <v>45605</v>
       </c>
-      <c r="O16" s="13"/>
+      <c r="O16" s="12"/>
       <c r="P16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="13"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="T16" s="21"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="T16" s="12"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="W16" s="12"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="15" t="s">
+      <c r="W16" s="21"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z16" s="16"/>
+      <c r="Z16" s="46"/>
       <c r="AA16" s="11"/>
-      <c r="AB16" s="13"/>
+      <c r="AB16" s="12"/>
     </row>
     <row r="17" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1578,20 +1578,20 @@
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="9">
+      <c r="M17" s="8">
         <v>45577</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="22">
         <v>45607</v>
       </c>
-      <c r="O17" s="13"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
@@ -1600,154 +1600,154 @@
       </c>
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
-      <c r="Y17" s="15" t="s">
+      <c r="Y17" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="16"/>
+      <c r="Z17" s="46"/>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
     </row>
     <row r="18" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="6"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="13"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="11"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="13"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="11"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="13"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="12"/>
       <c r="V18" s="11"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z18" s="48"/>
       <c r="AA18" s="11">
         <v>2</v>
       </c>
-      <c r="AB18" s="13"/>
+      <c r="AB18" s="12"/>
     </row>
     <row r="19" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
+        <v>61</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="6"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="5"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="13"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="11"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="13"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="11"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="13"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="12"/>
       <c r="V19" s="11"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z19" s="48"/>
       <c r="AA19" s="11">
         <v>2</v>
       </c>
-      <c r="AB19" s="13"/>
+      <c r="AB19" s="12"/>
     </row>
     <row r="20" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13"/>
+        <v>60</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="6"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="11"/>
-      <c r="O20" s="13"/>
+      <c r="O20" s="12"/>
       <c r="P20" s="11"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="13"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="11"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="13"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="12"/>
       <c r="V20" s="11"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z20" s="48"/>
       <c r="AA20" s="11">
         <v>2</v>
       </c>
-      <c r="AB20" s="13"/>
+      <c r="AB20" s="12"/>
     </row>
     <row r="21" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="6"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="11"/>
-      <c r="O21" s="13"/>
+      <c r="O21" s="12"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="13"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="12"/>
       <c r="S21" s="11"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="13"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="12"/>
       <c r="V21" s="11"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z21" s="48"/>
       <c r="AA21" s="11">
         <v>2</v>
       </c>
-      <c r="AB21" s="13"/>
+      <c r="AB21" s="12"/>
     </row>
     <row r="22" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="42"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="14" t="s">
         <v>21</v>
       </c>
@@ -1760,10 +1760,10 @@
       </c>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="3">
+      <c r="M22" s="2">
         <v>45590</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="13">
         <v>45590</v>
       </c>
       <c r="O22" s="14"/>
@@ -1782,16 +1782,16 @@
       </c>
       <c r="W22" s="14"/>
       <c r="X22" s="14"/>
-      <c r="Y22" s="15" t="s">
+      <c r="Y22" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z22" s="16"/>
+      <c r="Z22" s="46"/>
       <c r="AA22" s="14"/>
       <c r="AB22" s="14"/>
     </row>
     <row r="23" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="14" t="s">
         <v>45</v>
       </c>
@@ -1804,10 +1804,10 @@
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="3">
+      <c r="M23" s="2">
         <v>45590</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23" s="13">
         <v>45590</v>
       </c>
       <c r="O23" s="14"/>
@@ -1826,16 +1826,16 @@
       </c>
       <c r="W23" s="14"/>
       <c r="X23" s="14"/>
-      <c r="Y23" s="15" t="s">
+      <c r="Y23" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z23" s="16"/>
+      <c r="Z23" s="46"/>
       <c r="AA23" s="14"/>
       <c r="AB23" s="14"/>
     </row>
     <row r="24" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="14" t="s">
         <v>41</v>
       </c>
@@ -1844,14 +1844,14 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="5">
+      <c r="M24" s="4">
         <v>45591</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="13">
         <v>45591</v>
       </c>
       <c r="O24" s="14"/>
@@ -1861,25 +1861,25 @@
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
       <c r="S24" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
       <c r="V24" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W24" s="14"/>
       <c r="X24" s="14"/>
-      <c r="Y24" s="15" t="s">
+      <c r="Y24" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z24" s="16"/>
+      <c r="Z24" s="46"/>
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
     </row>
     <row r="25" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C25" s="43"/>
-      <c r="D25" s="44"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="14" t="s">
         <v>42</v>
       </c>
@@ -1892,10 +1892,10 @@
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <v>45595</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25" s="13">
         <v>45608</v>
       </c>
       <c r="O25" s="14"/>
@@ -1910,20 +1910,20 @@
       <c r="T25" s="14"/>
       <c r="U25" s="14"/>
       <c r="V25" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W25" s="14"/>
       <c r="X25" s="14"/>
-      <c r="Y25" s="15" t="s">
+      <c r="Y25" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="16"/>
+      <c r="Z25" s="46"/>
       <c r="AA25" s="14"/>
       <c r="AB25" s="14"/>
     </row>
     <row r="26" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="14" t="s">
         <v>44</v>
       </c>
@@ -1936,10 +1936,10 @@
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="9">
+      <c r="M26" s="8">
         <v>45597</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26" s="13">
         <v>45603</v>
       </c>
       <c r="O26" s="14"/>
@@ -1949,149 +1949,159 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T26" s="14"/>
       <c r="U26" s="14"/>
       <c r="V26" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W26" s="14"/>
       <c r="X26" s="14"/>
-      <c r="Y26" s="15" t="s">
+      <c r="Y26" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="16"/>
+      <c r="Z26" s="46"/>
       <c r="AA26" s="14"/>
       <c r="AB26" s="14"/>
     </row>
     <row r="27" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="14" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="J27" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="14"/>
+      <c r="M27" s="10">
+        <v>45595</v>
+      </c>
+      <c r="N27" s="13">
+        <v>45608</v>
+      </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
+      <c r="P27" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="S27" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="T27" s="14"/>
       <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
+      <c r="V27" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="W27" s="14"/>
       <c r="X27" s="14"/>
-      <c r="Y27" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="14">
-        <v>1</v>
-      </c>
+      <c r="Y27" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z27" s="46"/>
+      <c r="AA27" s="14"/>
       <c r="AB27" s="14"/>
     </row>
     <row r="28" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
       <c r="E28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
+        <v>54</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="12"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="10">
+      <c r="K28" s="21"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="9">
         <v>45608</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="22">
         <v>45608</v>
       </c>
-      <c r="O28" s="13"/>
+      <c r="O28" s="12"/>
       <c r="P28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="13"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="12"/>
       <c r="S28" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="T28" s="12"/>
-      <c r="U28" s="13"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="12"/>
       <c r="V28" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
-      <c r="Y28" s="15" t="s">
+      <c r="Y28" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z28" s="16"/>
+      <c r="Z28" s="46"/>
       <c r="AA28" s="14"/>
       <c r="AB28" s="14"/>
     </row>
     <row r="29" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
       <c r="E29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="12"/>
       <c r="J29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="12"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="10">
+      <c r="K29" s="21"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="9">
         <v>45608</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="22">
         <v>45608</v>
       </c>
-      <c r="O29" s="13"/>
+      <c r="O29" s="12"/>
       <c r="P29" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="13"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="12"/>
       <c r="S29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="T29" s="12"/>
-      <c r="U29" s="13"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="12"/>
       <c r="V29" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W29" s="14"/>
       <c r="X29" s="14"/>
-      <c r="Y29" s="15" t="s">
+      <c r="Y29" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z29" s="16"/>
+      <c r="Z29" s="46"/>
       <c r="AA29" s="14"/>
       <c r="AB29" s="14"/>
     </row>
     <row r="30" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
       <c r="E30" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -2102,10 +2112,10 @@
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="9">
+      <c r="M30" s="8">
         <v>45597</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="13">
         <v>45603</v>
       </c>
       <c r="O30" s="14"/>
@@ -2115,61 +2125,61 @@
       <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
       <c r="S30" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
       <c r="V30" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W30" s="14"/>
       <c r="X30" s="14"/>
-      <c r="Y30" s="15" t="s">
+      <c r="Y30" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="16"/>
+      <c r="Z30" s="46"/>
       <c r="AA30" s="14"/>
       <c r="AB30" s="14"/>
     </row>
     <row r="31" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="13"/>
+        <v>62</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="12"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="6"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="5"/>
       <c r="N31" s="11"/>
-      <c r="O31" s="13"/>
+      <c r="O31" s="12"/>
       <c r="P31" s="11"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="13"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="12"/>
       <c r="S31" s="11"/>
-      <c r="T31" s="12"/>
-      <c r="U31" s="13"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="12"/>
       <c r="V31" s="11"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z31" s="48"/>
       <c r="AA31" s="11">
         <v>2</v>
       </c>
-      <c r="AB31" s="13"/>
+      <c r="AB31" s="12"/>
     </row>
     <row r="32" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="34"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="14" t="s">
         <v>43</v>
       </c>
@@ -2182,10 +2192,10 @@
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
-      <c r="M32" s="5">
+      <c r="M32" s="4">
         <v>45595</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="13">
         <v>45600</v>
       </c>
       <c r="O32" s="14"/>
@@ -2200,22 +2210,22 @@
       <c r="T32" s="14"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W32" s="14"/>
       <c r="X32" s="14"/>
-      <c r="Y32" s="15" t="s">
+      <c r="Y32" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z32" s="16"/>
+      <c r="Z32" s="46"/>
       <c r="AA32" s="14"/>
       <c r="AB32" s="14"/>
     </row>
     <row r="33" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -2226,10 +2236,10 @@
       </c>
       <c r="K33" s="14"/>
       <c r="L33" s="14"/>
-      <c r="M33" s="5">
+      <c r="M33" s="4">
         <v>45595</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="13">
         <v>45597</v>
       </c>
       <c r="O33" s="14"/>
@@ -2244,37 +2254,263 @@
       <c r="T33" s="14"/>
       <c r="U33" s="14"/>
       <c r="V33" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W33" s="14"/>
       <c r="X33" s="14"/>
-      <c r="Y33" s="15" t="s">
+      <c r="Y33" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z33" s="16"/>
+      <c r="Z33" s="46"/>
       <c r="AA33" s="14"/>
       <c r="AB33" s="14"/>
     </row>
     <row r="40" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC40" s="15" t="s">
+      <c r="AC40" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AD40" s="16"/>
+      <c r="AD40" s="46"/>
     </row>
     <row r="42" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC42" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD42" s="19"/>
+      <c r="AC42" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD42" s="51"/>
     </row>
     <row r="44" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC44" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD44" s="21"/>
+      <c r="AC44" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD44" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="250">
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="AA32:AB32"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="C3:AB3"/>
+    <mergeCell ref="AC40:AD40"/>
+    <mergeCell ref="AC42:AD42"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AA25:AB25"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="V32:X32"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="V24:X24"/>
+    <mergeCell ref="V25:X25"/>
+    <mergeCell ref="V26:X26"/>
+    <mergeCell ref="V27:X27"/>
+    <mergeCell ref="V30:X30"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="V20:X20"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="V31:X31"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="S32:U32"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="C5:D10"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="C17:D21"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C22:D31"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="AA31:AB31"/>
     <mergeCell ref="N30:O30"/>
     <mergeCell ref="AA26:AB26"/>
@@ -2299,232 +2535,6 @@
     <mergeCell ref="AA28:AB28"/>
     <mergeCell ref="AA29:AB29"/>
     <mergeCell ref="E28:I28"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="C5:D10"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="C17:D21"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C22:D31"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="S32:U32"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="V33:X33"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="V25:X25"/>
-    <mergeCell ref="V26:X26"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="V30:X30"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="V21:X21"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="V31:X31"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="V32:X32"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="AA32:AB32"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="C3:AB3"/>
-    <mergeCell ref="AC40:AD40"/>
-    <mergeCell ref="AC42:AD42"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AA25:AB25"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de la planificación 27/11/2024
</commit_message>
<xml_diff>
--- a/Gestión del Proyecto/Planificación.xlsx
+++ b/Gestión del Proyecto/Planificación.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>Planificación del trabajo Completa</t>
   </si>
@@ -252,9 +252,6 @@
     <t xml:space="preserve"> 1 Hora</t>
   </si>
   <si>
-    <t xml:space="preserve"> - 30 Minutos</t>
-  </si>
-  <si>
     <t>3 Horas (x4)</t>
   </si>
   <si>
@@ -273,13 +270,13 @@
     <t xml:space="preserve"> - 1 Hora </t>
   </si>
   <si>
-    <t>25 Minutos</t>
-  </si>
-  <si>
-    <t>5 Minutos</t>
-  </si>
-  <si>
     <t>Comunicación entre dos agentes (Prototipo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 Horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - 3 Horas</t>
   </si>
 </sst>
 </file>
@@ -528,14 +525,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,102 +647,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,7 +931,7 @@
   <dimension ref="C3:AD44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27:R27"/>
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,88 +945,88 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
     </row>
     <row r="4" spans="3:29" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="23" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
       <c r="M4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23" t="s">
+      <c r="O4" s="22"/>
+      <c r="P4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23" t="s">
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="49" t="s">
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="23" t="s">
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23" t="s">
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AB4" s="23"/>
+      <c r="AB4" s="22"/>
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1042,7 @@
       <c r="M5" s="2">
         <v>45576</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="24">
         <v>45576</v>
       </c>
       <c r="O5" s="14"/>
@@ -1064,17 +1061,17 @@
       </c>
       <c r="W5" s="14"/>
       <c r="X5" s="14"/>
-      <c r="Y5" s="45" t="s">
+      <c r="Y5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z5" s="46"/>
+      <c r="Z5" s="16"/>
       <c r="AA5" s="14"/>
       <c r="AB5" s="14"/>
       <c r="AC5" s="6"/>
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="14" t="s">
         <v>16</v>
       </c>
@@ -1090,17 +1087,17 @@
       <c r="M6" s="2">
         <v>45576</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="24">
         <v>45580</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
@@ -1109,16 +1106,16 @@
       </c>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
-      <c r="Y6" s="45" t="s">
+      <c r="Y6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="46"/>
+      <c r="Z6" s="16"/>
       <c r="AA6" s="14"/>
       <c r="AB6" s="14"/>
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="14" t="s">
         <v>37</v>
       </c>
@@ -1134,7 +1131,7 @@
       <c r="M7" s="2">
         <v>45582</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="24">
         <v>45590</v>
       </c>
       <c r="O7" s="14"/>
@@ -1153,61 +1150,61 @@
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
-      <c r="Y7" s="45" t="s">
+      <c r="Y7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z7" s="46"/>
+      <c r="Z7" s="16"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
       <c r="AC7" s="6"/>
     </row>
     <row r="8" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="3">
         <v>45576</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="23">
         <v>45589</v>
       </c>
-      <c r="O8" s="24"/>
+      <c r="O8" s="25"/>
       <c r="P8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="13"/>
       <c r="S8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="21"/>
-      <c r="U8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="13"/>
       <c r="V8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="W8" s="14"/>
       <c r="X8" s="14"/>
-      <c r="Y8" s="45" t="s">
+      <c r="Y8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="46"/>
+      <c r="Z8" s="16"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
@@ -1223,7 +1220,7 @@
       <c r="M9" s="2">
         <v>45576</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="24">
         <v>45590</v>
       </c>
       <c r="O9" s="14"/>
@@ -1242,64 +1239,64 @@
       </c>
       <c r="W9" s="14"/>
       <c r="X9" s="14"/>
-      <c r="Y9" s="45" t="s">
+      <c r="Y9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z9" s="46"/>
+      <c r="Z9" s="16"/>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
       <c r="AC9" s="6"/>
     </row>
     <row r="10" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
       <c r="M10" s="7">
         <v>45597</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="23">
         <v>45600</v>
       </c>
-      <c r="O10" s="24"/>
+      <c r="O10" s="25"/>
       <c r="P10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
       <c r="S10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="T10" s="12"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="W10" s="14"/>
       <c r="X10" s="14"/>
-      <c r="Y10" s="45" t="s">
+      <c r="Y10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z10" s="46"/>
+      <c r="Z10" s="16"/>
       <c r="AA10" s="11"/>
-      <c r="AB10" s="12"/>
+      <c r="AB10" s="13"/>
       <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="14" t="s">
         <v>53</v>
       </c>
@@ -1315,7 +1312,7 @@
       <c r="M11" s="8">
         <v>45577</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="24">
         <v>45608</v>
       </c>
       <c r="O11" s="14"/>
@@ -1325,25 +1322,25 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="S11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
-      <c r="Y11" s="45" t="s">
+      <c r="Y11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z11" s="46"/>
+      <c r="Z11" s="16"/>
       <c r="AA11" s="14"/>
       <c r="AB11" s="14"/>
     </row>
     <row r="12" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="14" t="s">
         <v>40</v>
       </c>
@@ -1359,7 +1356,7 @@
       <c r="M12" s="8">
         <v>45591</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="24">
         <v>45591</v>
       </c>
       <c r="O12" s="14"/>
@@ -1378,60 +1375,60 @@
       </c>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
-      <c r="Y12" s="45" t="s">
+      <c r="Y12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z12" s="46"/>
+      <c r="Z12" s="16"/>
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
     </row>
     <row r="13" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="8">
         <v>45597</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="23">
         <v>45597</v>
       </c>
-      <c r="O13" s="12"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="13"/>
       <c r="S13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="T13" s="21"/>
-      <c r="U13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="13"/>
       <c r="V13" s="14" t="s">
         <v>66</v>
       </c>
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
-      <c r="Y13" s="45" t="s">
+      <c r="Y13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z13" s="46"/>
+      <c r="Z13" s="16"/>
       <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
     </row>
     <row r="14" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="14" t="s">
         <v>47</v>
       </c>
@@ -1447,7 +1444,7 @@
       <c r="M14" s="8">
         <v>45591</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="24">
         <v>45591</v>
       </c>
       <c r="O14" s="14"/>
@@ -1466,106 +1463,106 @@
       </c>
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
-      <c r="Y14" s="45" t="s">
+      <c r="Y14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z14" s="46"/>
+      <c r="Z14" s="16"/>
       <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
     </row>
     <row r="15" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="8">
         <v>45577</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="23">
         <v>45604</v>
       </c>
-      <c r="O15" s="12"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="13"/>
       <c r="S15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="T15" s="21"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="W15" s="21"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="T15" s="12"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z15" s="46"/>
+      <c r="Z15" s="16"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="12"/>
+      <c r="AB15" s="13"/>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
       <c r="M16" s="8">
         <v>45577</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="23">
         <v>45605</v>
       </c>
-      <c r="O16" s="12"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="12"/>
+        <v>38</v>
+      </c>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13"/>
       <c r="S16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="W16" s="21"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="12"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z16" s="46"/>
+      <c r="Z16" s="16"/>
       <c r="AA16" s="11"/>
-      <c r="AB16" s="12"/>
+      <c r="AB16" s="13"/>
     </row>
     <row r="17" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="14" t="s">
         <v>48</v>
       </c>
@@ -1581,173 +1578,173 @@
       <c r="M17" s="8">
         <v>45577</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="23">
         <v>45607</v>
       </c>
-      <c r="O17" s="12"/>
+      <c r="O17" s="13"/>
       <c r="P17" s="14" t="s">
         <v>75</v>
       </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
       <c r="V17" s="14" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="W17" s="14"/>
       <c r="X17" s="14"/>
-      <c r="Y17" s="45" t="s">
+      <c r="Y17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="46"/>
+      <c r="Z17" s="16"/>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
     </row>
     <row r="18" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="5"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="12"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="11"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13"/>
       <c r="S18" s="11"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="13"/>
       <c r="V18" s="11"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="47" t="s">
+      <c r="W18" s="12"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Z18" s="48"/>
+      <c r="Z18" s="21"/>
       <c r="AA18" s="11">
         <v>2</v>
       </c>
-      <c r="AB18" s="12"/>
+      <c r="AB18" s="13"/>
     </row>
     <row r="19" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
       <c r="M19" s="5"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="12"/>
+      <c r="O19" s="13"/>
       <c r="P19" s="11"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13"/>
       <c r="S19" s="11"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="13"/>
       <c r="V19" s="11"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="47" t="s">
+      <c r="W19" s="12"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Z19" s="48"/>
+      <c r="Z19" s="21"/>
       <c r="AA19" s="11">
         <v>2</v>
       </c>
-      <c r="AB19" s="12"/>
+      <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="5"/>
       <c r="N20" s="11"/>
-      <c r="O20" s="12"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="11"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="13"/>
       <c r="S20" s="11"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="13"/>
       <c r="V20" s="11"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="47" t="s">
+      <c r="W20" s="12"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Z20" s="48"/>
+      <c r="Z20" s="21"/>
       <c r="AA20" s="11">
         <v>2</v>
       </c>
-      <c r="AB20" s="12"/>
+      <c r="AB20" s="13"/>
     </row>
     <row r="21" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="5"/>
       <c r="N21" s="11"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="13"/>
       <c r="S21" s="11"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="13"/>
       <c r="V21" s="11"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="47" t="s">
+      <c r="W21" s="12"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Z21" s="48"/>
+      <c r="Z21" s="21"/>
       <c r="AA21" s="11">
         <v>2</v>
       </c>
-      <c r="AB21" s="12"/>
+      <c r="AB21" s="13"/>
     </row>
     <row r="22" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="14" t="s">
         <v>21</v>
       </c>
@@ -1763,7 +1760,7 @@
       <c r="M22" s="2">
         <v>45590</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="24">
         <v>45590</v>
       </c>
       <c r="O22" s="14"/>
@@ -1782,16 +1779,16 @@
       </c>
       <c r="W22" s="14"/>
       <c r="X22" s="14"/>
-      <c r="Y22" s="45" t="s">
+      <c r="Y22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z22" s="46"/>
+      <c r="Z22" s="16"/>
       <c r="AA22" s="14"/>
       <c r="AB22" s="14"/>
     </row>
     <row r="23" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="14" t="s">
         <v>45</v>
       </c>
@@ -1807,7 +1804,7 @@
       <c r="M23" s="2">
         <v>45590</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="24">
         <v>45590</v>
       </c>
       <c r="O23" s="14"/>
@@ -1826,16 +1823,16 @@
       </c>
       <c r="W23" s="14"/>
       <c r="X23" s="14"/>
-      <c r="Y23" s="45" t="s">
+      <c r="Y23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z23" s="46"/>
+      <c r="Z23" s="16"/>
       <c r="AA23" s="14"/>
       <c r="AB23" s="14"/>
     </row>
     <row r="24" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="14" t="s">
         <v>41</v>
       </c>
@@ -1851,7 +1848,7 @@
       <c r="M24" s="4">
         <v>45591</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="24">
         <v>45591</v>
       </c>
       <c r="O24" s="14"/>
@@ -1870,16 +1867,16 @@
       </c>
       <c r="W24" s="14"/>
       <c r="X24" s="14"/>
-      <c r="Y24" s="45" t="s">
+      <c r="Y24" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z24" s="46"/>
+      <c r="Z24" s="16"/>
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
     </row>
     <row r="25" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="14" t="s">
         <v>42</v>
       </c>
@@ -1895,7 +1892,7 @@
       <c r="M25" s="9">
         <v>45595</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="24">
         <v>45608</v>
       </c>
       <c r="O25" s="14"/>
@@ -1914,16 +1911,16 @@
       </c>
       <c r="W25" s="14"/>
       <c r="X25" s="14"/>
-      <c r="Y25" s="45" t="s">
+      <c r="Y25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="46"/>
+      <c r="Z25" s="16"/>
       <c r="AA25" s="14"/>
       <c r="AB25" s="14"/>
     </row>
     <row r="26" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="14" t="s">
         <v>44</v>
       </c>
@@ -1939,7 +1936,7 @@
       <c r="M26" s="8">
         <v>45597</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="24">
         <v>45603</v>
       </c>
       <c r="O26" s="14"/>
@@ -1958,18 +1955,18 @@
       </c>
       <c r="W26" s="14"/>
       <c r="X26" s="14"/>
-      <c r="Y26" s="45" t="s">
+      <c r="Y26" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="46"/>
+      <c r="Z26" s="16"/>
       <c r="AA26" s="14"/>
       <c r="AB26" s="14"/>
     </row>
     <row r="27" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1983,12 +1980,12 @@
       <c r="M27" s="10">
         <v>45595</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="24">
         <v>45608</v>
       </c>
       <c r="O27" s="14"/>
       <c r="P27" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
@@ -2002,104 +1999,104 @@
       </c>
       <c r="W27" s="14"/>
       <c r="X27" s="14"/>
-      <c r="Y27" s="45" t="s">
+      <c r="Y27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z27" s="46"/>
+      <c r="Z27" s="16"/>
       <c r="AA27" s="14"/>
       <c r="AB27" s="14"/>
     </row>
     <row r="28" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="21"/>
-      <c r="L28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
       <c r="M28" s="9">
         <v>45608</v>
       </c>
-      <c r="N28" s="22">
+      <c r="N28" s="23">
         <v>45608</v>
       </c>
-      <c r="O28" s="12"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="13"/>
       <c r="S28" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="T28" s="21"/>
-      <c r="U28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="13"/>
       <c r="V28" s="14" t="s">
         <v>76</v>
       </c>
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
-      <c r="Y28" s="45" t="s">
+      <c r="Y28" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z28" s="46"/>
+      <c r="Z28" s="16"/>
       <c r="AA28" s="14"/>
       <c r="AB28" s="14"/>
     </row>
     <row r="29" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
       <c r="E29" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="13"/>
       <c r="M29" s="9">
         <v>45608</v>
       </c>
-      <c r="N29" s="22">
+      <c r="N29" s="23">
         <v>45608</v>
       </c>
-      <c r="O29" s="12"/>
+      <c r="O29" s="13"/>
       <c r="P29" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="13"/>
       <c r="S29" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="T29" s="21"/>
-      <c r="U29" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="T29" s="12"/>
+      <c r="U29" s="13"/>
       <c r="V29" s="14" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="W29" s="14"/>
       <c r="X29" s="14"/>
-      <c r="Y29" s="45" t="s">
+      <c r="Y29" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z29" s="46"/>
+      <c r="Z29" s="16"/>
       <c r="AA29" s="14"/>
       <c r="AB29" s="14"/>
     </row>
     <row r="30" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
       <c r="E30" s="14" t="s">
         <v>46</v>
       </c>
@@ -2115,7 +2112,7 @@
       <c r="M30" s="8">
         <v>45597</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="24">
         <v>45603</v>
       </c>
       <c r="O30" s="14"/>
@@ -2134,52 +2131,52 @@
       </c>
       <c r="W30" s="14"/>
       <c r="X30" s="14"/>
-      <c r="Y30" s="45" t="s">
+      <c r="Y30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="46"/>
+      <c r="Z30" s="16"/>
       <c r="AA30" s="14"/>
       <c r="AB30" s="14"/>
     </row>
     <row r="31" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="13"/>
       <c r="M31" s="5"/>
       <c r="N31" s="11"/>
-      <c r="O31" s="12"/>
+      <c r="O31" s="13"/>
       <c r="P31" s="11"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="13"/>
       <c r="S31" s="11"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="13"/>
       <c r="V31" s="11"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="12"/>
-      <c r="Y31" s="47" t="s">
+      <c r="W31" s="12"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Z31" s="48"/>
+      <c r="Z31" s="21"/>
       <c r="AA31" s="11">
         <v>2</v>
       </c>
-      <c r="AB31" s="12"/>
+      <c r="AB31" s="13"/>
     </row>
     <row r="32" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="14" t="s">
         <v>43</v>
       </c>
@@ -2195,7 +2192,7 @@
       <c r="M32" s="4">
         <v>45595</v>
       </c>
-      <c r="N32" s="13">
+      <c r="N32" s="24">
         <v>45600</v>
       </c>
       <c r="O32" s="14"/>
@@ -2214,16 +2211,16 @@
       </c>
       <c r="W32" s="14"/>
       <c r="X32" s="14"/>
-      <c r="Y32" s="45" t="s">
+      <c r="Y32" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z32" s="46"/>
+      <c r="Z32" s="16"/>
       <c r="AA32" s="14"/>
       <c r="AB32" s="14"/>
     </row>
     <row r="33" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="14" t="s">
         <v>49</v>
       </c>
@@ -2239,7 +2236,7 @@
       <c r="M33" s="4">
         <v>45595</v>
       </c>
-      <c r="N33" s="13">
+      <c r="N33" s="24">
         <v>45597</v>
       </c>
       <c r="O33" s="14"/>
@@ -2258,42 +2255,250 @@
       </c>
       <c r="W33" s="14"/>
       <c r="X33" s="14"/>
-      <c r="Y33" s="45" t="s">
+      <c r="Y33" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Z33" s="46"/>
+      <c r="Z33" s="16"/>
       <c r="AA33" s="14"/>
       <c r="AB33" s="14"/>
     </row>
     <row r="40" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC40" s="45" t="s">
+      <c r="AC40" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AD40" s="46"/>
+      <c r="AD40" s="16"/>
     </row>
     <row r="42" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC42" s="50" t="s">
+      <c r="AC42" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="AD42" s="51"/>
+      <c r="AD42" s="19"/>
     </row>
     <row r="44" spans="3:30" x14ac:dyDescent="0.3">
-      <c r="AC44" s="47" t="s">
+      <c r="AC44" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AD44" s="48"/>
+      <c r="AD44" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="250">
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="AA27:AB27"/>
+    <mergeCell ref="C11:D16"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="AA28:AB28"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="C5:D10"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="C17:D21"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C22:D31"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="S32:U32"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="S21:U21"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="S31:U31"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="V24:X24"/>
+    <mergeCell ref="V25:X25"/>
+    <mergeCell ref="V26:X26"/>
+    <mergeCell ref="V27:X27"/>
+    <mergeCell ref="V30:X30"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="V20:X20"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="V21:X21"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="V31:X31"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="V32:X32"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="V8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="S30:U30"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA30:AB30"/>
     <mergeCell ref="AA32:AB32"/>
     <mergeCell ref="AA33:AB33"/>
     <mergeCell ref="C3:AB3"/>
@@ -2318,223 +2523,15 @@
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="J17:L17"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="V8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="S30:U30"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="V32:X32"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="V33:X33"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="V25:X25"/>
-    <mergeCell ref="V26:X26"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="V30:X30"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="V21:X21"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="V31:X31"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="S32:U32"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S31:U31"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="C5:D10"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="C17:D21"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C22:D31"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="AA27:AB27"/>
-    <mergeCell ref="C11:D16"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="AA28:AB28"/>
-    <mergeCell ref="AA29:AB29"/>
-    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>